<commit_message>
Fix bugs on auto-register
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75CF139-50DB-40BC-8B59-7C75A9AF7CFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C682B40-8C41-4DC1-AD06-CD5ADFB5DB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
@@ -53,21 +53,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Finish auto register script in Python</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Used Selenium, chrome driver, excel read and write, multiprocessing-Pool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reminder to modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. make sure the input excel sheet with the proper name same as the village name;
-2. ban the register function before formal running, test the read and write Excel process;
-3. remove the user data after registration and avoid upload it github</t>
+    <t>Run auto register script with real data and fix some bugs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>learn Python data types: string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>learned by Think like a computer scientist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Didn't find the root cause why the browser opened more than 8 while I set Pool size to 8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -523,7 +521,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -544,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -552,15 +550,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="6"/>
@@ -578,16 +580,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">

</xml_diff>

<commit_message>
learned high-features and functions
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C682B40-8C41-4DC1-AD06-CD5ADFB5DB61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D72B8D5-74A1-4A1C-9AD5-03DCE1766833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
+    <workbookView xWindow="7365" yWindow="5078" windowWidth="16875" windowHeight="10515" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,19 +53,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Run auto register script with real data and fix some bugs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>learn Python data types: string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>learned by Think like a computer scientist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Didn't find the root cause why the browser opened more than 8 while I set Pool size to 8</t>
+    <t>Including iteration(Iterable, Iterator) and generator, list generator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>learned high-level features</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">learned high-level function </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Including return function(return value is a function), lambda function, decorator, partial function, high-level built-in functions like map/reduce and filter, sorted</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,7 +521,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -542,26 +542,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
April 22, high-level features of OOP
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D72B8D5-74A1-4A1C-9AD5-03DCE1766833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA839C05-840B-49F5-9F9E-D007A11A7B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="5078" windowWidth="16875" windowHeight="10515" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
+    <workbookView xWindow="5393" yWindow="1920" windowWidth="16875" windowHeight="10515" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,19 +53,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Including iteration(Iterable, Iterator) and generator, list generator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>learned high-level features</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">learned high-level function </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Including return function(return value is a function), lambda function, decorator, partial function, high-level built-in functions like map/reduce and filter, sorted</t>
+    <t>learned high-level OOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Including __slots__, @property, multi-inheritation, customized class, Enum class, metaclass;
+Use of exception handling: try, except and finally, raise Exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recalled OOP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,7 +518,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -547,21 +544,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="40.5" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
learn debug,test and file operation, serialization
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA839C05-840B-49F5-9F9E-D007A11A7B6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD16A0B-121E-4E1A-B35E-953D47A13DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5393" yWindow="1920" windowWidth="16875" windowHeight="10515" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
+    <workbookView xWindow="4350" yWindow="1298" windowWidth="16875" windowHeight="10515" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,16 +53,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>learned high-level OOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Including __slots__, @property, multi-inheritation, customized class, Enum class, metaclass;
-Use of exception handling: try, except and finally, raise Exception</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Recalled OOP</t>
+    <t>Learned debug and test module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>including debug, unittest, doctest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>learned IO programming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Including file read/write and file and directory operation, serialization using json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -544,19 +547,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="40.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
learned basic algorithms to Dijkstra
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD16A0B-121E-4E1A-B35E-953D47A13DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CFDA20-AF09-409B-99D7-05082E5129A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="1298" windowWidth="16875" windowHeight="10515" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
+    <workbookView xWindow="6548" yWindow="2528" windowWidth="16875" windowHeight="10522" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,19 +53,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Learned debug and test module</t>
+    <t>learned algorithms with implement programing at same time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>including debug, unittest, doctest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>learned IO programming</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Including file read/write and file and directory operation, serialization using json</t>
+    <t>Including algorithm basics, like capital O representation method, binary search, selection sort, recursive, quick sort, hash table, BFS, Dijkstra algorithm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -176,7 +168,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -194,6 +186,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -518,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B28C9F-318C-44C4-B0BD-00C62A359313}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -542,7 +543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -557,46 +558,49 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
learned greedy alrorithm and bag problem of dynamic plan
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CFDA20-AF09-409B-99D7-05082E5129A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733D14F7-2A3E-4F37-B464-75C4D5686E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6548" yWindow="2528" windowWidth="16875" windowHeight="10522" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
+    <workbookView xWindow="1448" yWindow="1995" windowWidth="16874" windowHeight="10522" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,7 +57,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Including algorithm basics, like capital O representation method, binary search, selection sort, recursive, quick sort, hash table, BFS, Dijkstra algorithm</t>
+    <t>Implement greedy algorithm, the bag problem of the dynamic plan;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go through the concept of several classifier, like KNN, Naïve Bayes, and introduction of other common and important algorithms, like MapReduce (distributed algorithm)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -102,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -162,13 +166,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -203,6 +233,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,7 +558,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -543,28 +579,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
+    <row r="2" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+    <row r="3" spans="1:3" ht="27" x14ac:dyDescent="0.4">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
+      <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
     </row>
@@ -599,8 +633,10 @@
       <c r="C8" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2nd time interview by R&D - April 29
</commit_message>
<xml_diff>
--- a/Daily Reports/Daily Report - Template.xlsx
+++ b/Daily Reports/Daily Report - Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Daily Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733D14F7-2A3E-4F37-B464-75C4D5686E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A32081-CF9D-416C-9BB7-9FE302604DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1448" yWindow="1995" windowWidth="16874" windowHeight="10522" xr2:uid="{70FC5AAC-8B91-47A2-80CE-56A23C59660A}"/>
   </bookViews>
@@ -53,15 +53,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>learned algorithms with implement programing at same time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Implement greedy algorithm, the bag problem of the dynamic plan;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Go through the concept of several classifier, like KNN, Naïve Bayes, and introduction of other common and important algorithms, like MapReduce (distributed algorithm)</t>
+    <t>learned HTTP and web development</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reviewed the learning notes in the past 2 weeks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Take the interview by VT department R&amp;D representative</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -106,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -166,39 +166,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -217,29 +191,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,7 +526,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -580,32 +548,36 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="12">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="27" x14ac:dyDescent="0.4">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="27" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
@@ -633,10 +605,8 @@
       <c r="C8" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>